<commit_message>
added buttons for task 5 and 6
</commit_message>
<xml_diff>
--- a/ComputersFactory/Excel-Reports/ComputerTypes.xlsx
+++ b/ComputersFactory/Excel-Reports/ComputerTypes.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet sheetId="2" r:id="rId2" name="Sheet2"/>
+    <sheet sheetId="3" r:id="rId3" name="Sheet3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -359,21 +359,345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>All in one</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>